<commit_message>
Update performance dashboard 2025-12-24 23:49 - Simplified Design
</commit_message>
<xml_diff>
--- a/performance-dashboard/archive/Trading_Performance_20251224.xlsx
+++ b/performance-dashboard/archive/Trading_Performance_20251224.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O16"/>
+  <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -504,10 +504,15 @@
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
+          <t>Files Count</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
           <t>Analysis Date</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Data Date</t>
         </is>
@@ -546,7 +551,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>+464.39%</t>
+          <t>+216.99%</t>
         </is>
       </c>
       <c r="H2" t="n">
@@ -573,14 +578,17 @@
         </is>
       </c>
       <c r="M2" t="n">
-        <v>4</v>
-      </c>
-      <c r="N2" t="inlineStr">
+        <v>6</v>
+      </c>
+      <c r="N2" t="n">
+        <v>6</v>
+      </c>
+      <c r="O2" t="inlineStr">
         <is>
           <t>2025-12-24</t>
         </is>
       </c>
-      <c r="O2" t="inlineStr">
+      <c r="P2" t="inlineStr">
         <is>
           <t>20251224</t>
         </is>
@@ -619,7 +627,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>+408.99%</t>
+          <t>+195.90%</t>
         </is>
       </c>
       <c r="H3" t="n">
@@ -646,14 +654,17 @@
         </is>
       </c>
       <c r="M3" t="n">
-        <v>4</v>
-      </c>
-      <c r="N3" t="inlineStr">
+        <v>6</v>
+      </c>
+      <c r="N3" t="n">
+        <v>6</v>
+      </c>
+      <c r="O3" t="inlineStr">
         <is>
           <t>2025-12-24</t>
         </is>
       </c>
-      <c r="O3" t="inlineStr">
+      <c r="P3" t="inlineStr">
         <is>
           <t>20251224</t>
         </is>
@@ -692,7 +703,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>+86.42%</t>
+          <t>+51.47%</t>
         </is>
       </c>
       <c r="H4" t="n">
@@ -719,14 +730,17 @@
         </is>
       </c>
       <c r="M4" t="n">
-        <v>4</v>
-      </c>
-      <c r="N4" t="inlineStr">
+        <v>6</v>
+      </c>
+      <c r="N4" t="n">
+        <v>6</v>
+      </c>
+      <c r="O4" t="inlineStr">
         <is>
           <t>2025-12-24</t>
         </is>
       </c>
-      <c r="O4" t="inlineStr">
+      <c r="P4" t="inlineStr">
         <is>
           <t>20251224</t>
         </is>
@@ -765,7 +779,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>+53.67%</t>
+          <t>+33.17%</t>
         </is>
       </c>
       <c r="H5" t="n">
@@ -792,14 +806,17 @@
         </is>
       </c>
       <c r="M5" t="n">
-        <v>4</v>
-      </c>
-      <c r="N5" t="inlineStr">
+        <v>6</v>
+      </c>
+      <c r="N5" t="n">
+        <v>6</v>
+      </c>
+      <c r="O5" t="inlineStr">
         <is>
           <t>2025-12-24</t>
         </is>
       </c>
-      <c r="O5" t="inlineStr">
+      <c r="P5" t="inlineStr">
         <is>
           <t>20251224</t>
         </is>
@@ -838,7 +855,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>+4.95%</t>
+          <t>+3.27%</t>
         </is>
       </c>
       <c r="H6" t="n">
@@ -865,14 +882,17 @@
         </is>
       </c>
       <c r="M6" t="n">
-        <v>4</v>
-      </c>
-      <c r="N6" t="inlineStr">
+        <v>6</v>
+      </c>
+      <c r="N6" t="n">
+        <v>6</v>
+      </c>
+      <c r="O6" t="inlineStr">
         <is>
           <t>2025-12-24</t>
         </is>
       </c>
-      <c r="O6" t="inlineStr">
+      <c r="P6" t="inlineStr">
         <is>
           <t>20251224</t>
         </is>
@@ -911,7 +931,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>+27.15%</t>
+          <t>+17.36%</t>
         </is>
       </c>
       <c r="H7" t="n">
@@ -938,14 +958,17 @@
         </is>
       </c>
       <c r="M7" t="n">
-        <v>4</v>
-      </c>
-      <c r="N7" t="inlineStr">
+        <v>6</v>
+      </c>
+      <c r="N7" t="n">
+        <v>6</v>
+      </c>
+      <c r="O7" t="inlineStr">
         <is>
           <t>2025-12-24</t>
         </is>
       </c>
-      <c r="O7" t="inlineStr">
+      <c r="P7" t="inlineStr">
         <is>
           <t>20251224</t>
         </is>
@@ -984,7 +1007,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>+200.18%</t>
+          <t>+108.09%</t>
         </is>
       </c>
       <c r="H8" t="n">
@@ -1011,14 +1034,17 @@
         </is>
       </c>
       <c r="M8" t="n">
-        <v>4</v>
-      </c>
-      <c r="N8" t="inlineStr">
+        <v>6</v>
+      </c>
+      <c r="N8" t="n">
+        <v>6</v>
+      </c>
+      <c r="O8" t="inlineStr">
         <is>
           <t>2025-12-24</t>
         </is>
       </c>
-      <c r="O8" t="inlineStr">
+      <c r="P8" t="inlineStr">
         <is>
           <t>20251224</t>
         </is>
@@ -1057,7 +1083,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>+27.65%</t>
+          <t>+17.68%</t>
         </is>
       </c>
       <c r="H9" t="n">
@@ -1084,14 +1110,17 @@
         </is>
       </c>
       <c r="M9" t="n">
-        <v>4</v>
-      </c>
-      <c r="N9" t="inlineStr">
+        <v>6</v>
+      </c>
+      <c r="N9" t="n">
+        <v>6</v>
+      </c>
+      <c r="O9" t="inlineStr">
         <is>
           <t>2025-12-24</t>
         </is>
       </c>
-      <c r="O9" t="inlineStr">
+      <c r="P9" t="inlineStr">
         <is>
           <t>20251224</t>
         </is>
@@ -1130,7 +1159,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>+9.06%</t>
+          <t>+5.95%</t>
         </is>
       </c>
       <c r="H10" t="n">
@@ -1157,14 +1186,17 @@
         </is>
       </c>
       <c r="M10" t="n">
-        <v>4</v>
-      </c>
-      <c r="N10" t="inlineStr">
+        <v>6</v>
+      </c>
+      <c r="N10" t="n">
+        <v>6</v>
+      </c>
+      <c r="O10" t="inlineStr">
         <is>
           <t>2025-12-24</t>
         </is>
       </c>
-      <c r="O10" t="inlineStr">
+      <c r="P10" t="inlineStr">
         <is>
           <t>20251224</t>
         </is>
@@ -1203,7 +1235,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>+3.23%</t>
+          <t>+2.14%</t>
         </is>
       </c>
       <c r="H11" t="n">
@@ -1230,14 +1262,17 @@
         </is>
       </c>
       <c r="M11" t="n">
-        <v>4</v>
-      </c>
-      <c r="N11" t="inlineStr">
+        <v>6</v>
+      </c>
+      <c r="N11" t="n">
+        <v>6</v>
+      </c>
+      <c r="O11" t="inlineStr">
         <is>
           <t>2025-12-24</t>
         </is>
       </c>
-      <c r="O11" t="inlineStr">
+      <c r="P11" t="inlineStr">
         <is>
           <t>20251224</t>
         </is>
@@ -1276,7 +1311,7 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>+21.66%</t>
+          <t>+16.98%</t>
         </is>
       </c>
       <c r="H12" t="n">
@@ -1303,14 +1338,17 @@
         </is>
       </c>
       <c r="M12" t="n">
-        <v>4</v>
-      </c>
-      <c r="N12" t="inlineStr">
+        <v>5</v>
+      </c>
+      <c r="N12" t="n">
+        <v>5</v>
+      </c>
+      <c r="O12" t="inlineStr">
         <is>
           <t>2025-12-24</t>
         </is>
       </c>
-      <c r="O12" t="inlineStr">
+      <c r="P12" t="inlineStr">
         <is>
           <t>20251223</t>
         </is>
@@ -1349,7 +1387,7 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>+259.97%</t>
+          <t>+134.88%</t>
         </is>
       </c>
       <c r="H13" t="n">
@@ -1376,14 +1414,17 @@
         </is>
       </c>
       <c r="M13" t="n">
-        <v>4</v>
-      </c>
-      <c r="N13" t="inlineStr">
+        <v>6</v>
+      </c>
+      <c r="N13" t="n">
+        <v>6</v>
+      </c>
+      <c r="O13" t="inlineStr">
         <is>
           <t>2025-12-24</t>
         </is>
       </c>
-      <c r="O13" t="inlineStr">
+      <c r="P13" t="inlineStr">
         <is>
           <t>20251224</t>
         </is>
@@ -1422,7 +1463,7 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>+240.85%</t>
+          <t>+126.49%</t>
         </is>
       </c>
       <c r="H14" t="n">
@@ -1449,14 +1490,17 @@
         </is>
       </c>
       <c r="M14" t="n">
-        <v>4</v>
-      </c>
-      <c r="N14" t="inlineStr">
+        <v>6</v>
+      </c>
+      <c r="N14" t="n">
+        <v>6</v>
+      </c>
+      <c r="O14" t="inlineStr">
         <is>
           <t>2025-12-24</t>
         </is>
       </c>
-      <c r="O14" t="inlineStr">
+      <c r="P14" t="inlineStr">
         <is>
           <t>20251224</t>
         </is>
@@ -1495,7 +1539,7 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>+5.55%</t>
+          <t>+3.66%</t>
         </is>
       </c>
       <c r="H15" t="n">
@@ -1522,14 +1566,17 @@
         </is>
       </c>
       <c r="M15" t="n">
-        <v>4</v>
-      </c>
-      <c r="N15" t="inlineStr">
+        <v>6</v>
+      </c>
+      <c r="N15" t="n">
+        <v>6</v>
+      </c>
+      <c r="O15" t="inlineStr">
         <is>
           <t>2025-12-24</t>
         </is>
       </c>
-      <c r="O15" t="inlineStr">
+      <c r="P15" t="inlineStr">
         <is>
           <t>20251224</t>
         </is>
@@ -1568,7 +1615,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>+64.91%</t>
+          <t>+39.58%</t>
         </is>
       </c>
       <c r="H16" t="n">
@@ -1595,14 +1642,17 @@
         </is>
       </c>
       <c r="M16" t="n">
-        <v>4</v>
-      </c>
-      <c r="N16" t="inlineStr">
+        <v>6</v>
+      </c>
+      <c r="N16" t="n">
+        <v>6</v>
+      </c>
+      <c r="O16" t="inlineStr">
         <is>
           <t>2025-12-24</t>
         </is>
       </c>
-      <c r="O16" t="inlineStr">
+      <c r="P16" t="inlineStr">
         <is>
           <t>20251224</t>
         </is>
@@ -1619,7 +1669,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O6"/>
+  <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1695,10 +1745,15 @@
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
+          <t>Files Count</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
           <t>Analysis Date</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Data Date</t>
         </is>
@@ -1737,7 +1792,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>+464.39%</t>
+          <t>+216.99%</t>
         </is>
       </c>
       <c r="H2" t="n">
@@ -1764,14 +1819,17 @@
         </is>
       </c>
       <c r="M2" t="n">
-        <v>4</v>
-      </c>
-      <c r="N2" t="inlineStr">
+        <v>6</v>
+      </c>
+      <c r="N2" t="n">
+        <v>6</v>
+      </c>
+      <c r="O2" t="inlineStr">
         <is>
           <t>2025-12-24</t>
         </is>
       </c>
-      <c r="O2" t="inlineStr">
+      <c r="P2" t="inlineStr">
         <is>
           <t>20251224</t>
         </is>
@@ -1810,7 +1868,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>+408.99%</t>
+          <t>+195.90%</t>
         </is>
       </c>
       <c r="H3" t="n">
@@ -1837,14 +1895,17 @@
         </is>
       </c>
       <c r="M3" t="n">
-        <v>4</v>
-      </c>
-      <c r="N3" t="inlineStr">
+        <v>6</v>
+      </c>
+      <c r="N3" t="n">
+        <v>6</v>
+      </c>
+      <c r="O3" t="inlineStr">
         <is>
           <t>2025-12-24</t>
         </is>
       </c>
-      <c r="O3" t="inlineStr">
+      <c r="P3" t="inlineStr">
         <is>
           <t>20251224</t>
         </is>
@@ -1883,7 +1944,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>+86.42%</t>
+          <t>+51.47%</t>
         </is>
       </c>
       <c r="H4" t="n">
@@ -1910,14 +1971,17 @@
         </is>
       </c>
       <c r="M4" t="n">
-        <v>4</v>
-      </c>
-      <c r="N4" t="inlineStr">
+        <v>6</v>
+      </c>
+      <c r="N4" t="n">
+        <v>6</v>
+      </c>
+      <c r="O4" t="inlineStr">
         <is>
           <t>2025-12-24</t>
         </is>
       </c>
-      <c r="O4" t="inlineStr">
+      <c r="P4" t="inlineStr">
         <is>
           <t>20251224</t>
         </is>
@@ -1956,7 +2020,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>+53.67%</t>
+          <t>+33.17%</t>
         </is>
       </c>
       <c r="H5" t="n">
@@ -1983,14 +2047,17 @@
         </is>
       </c>
       <c r="M5" t="n">
-        <v>4</v>
-      </c>
-      <c r="N5" t="inlineStr">
+        <v>6</v>
+      </c>
+      <c r="N5" t="n">
+        <v>6</v>
+      </c>
+      <c r="O5" t="inlineStr">
         <is>
           <t>2025-12-24</t>
         </is>
       </c>
-      <c r="O5" t="inlineStr">
+      <c r="P5" t="inlineStr">
         <is>
           <t>20251224</t>
         </is>
@@ -2029,7 +2096,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>+4.95%</t>
+          <t>+3.27%</t>
         </is>
       </c>
       <c r="H6" t="n">
@@ -2056,14 +2123,17 @@
         </is>
       </c>
       <c r="M6" t="n">
-        <v>4</v>
-      </c>
-      <c r="N6" t="inlineStr">
+        <v>6</v>
+      </c>
+      <c r="N6" t="n">
+        <v>6</v>
+      </c>
+      <c r="O6" t="inlineStr">
         <is>
           <t>2025-12-24</t>
         </is>
       </c>
-      <c r="O6" t="inlineStr">
+      <c r="P6" t="inlineStr">
         <is>
           <t>20251224</t>
         </is>
@@ -2080,7 +2150,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O6"/>
+  <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2156,10 +2226,15 @@
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
+          <t>Files Count</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
           <t>Analysis Date</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Data Date</t>
         </is>
@@ -2198,7 +2273,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>+27.15%</t>
+          <t>+17.36%</t>
         </is>
       </c>
       <c r="H2" t="n">
@@ -2225,14 +2300,17 @@
         </is>
       </c>
       <c r="M2" t="n">
-        <v>4</v>
-      </c>
-      <c r="N2" t="inlineStr">
+        <v>6</v>
+      </c>
+      <c r="N2" t="n">
+        <v>6</v>
+      </c>
+      <c r="O2" t="inlineStr">
         <is>
           <t>2025-12-24</t>
         </is>
       </c>
-      <c r="O2" t="inlineStr">
+      <c r="P2" t="inlineStr">
         <is>
           <t>20251224</t>
         </is>
@@ -2271,7 +2349,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>+200.18%</t>
+          <t>+108.09%</t>
         </is>
       </c>
       <c r="H3" t="n">
@@ -2298,14 +2376,17 @@
         </is>
       </c>
       <c r="M3" t="n">
-        <v>4</v>
-      </c>
-      <c r="N3" t="inlineStr">
+        <v>6</v>
+      </c>
+      <c r="N3" t="n">
+        <v>6</v>
+      </c>
+      <c r="O3" t="inlineStr">
         <is>
           <t>2025-12-24</t>
         </is>
       </c>
-      <c r="O3" t="inlineStr">
+      <c r="P3" t="inlineStr">
         <is>
           <t>20251224</t>
         </is>
@@ -2344,7 +2425,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>+27.65%</t>
+          <t>+17.68%</t>
         </is>
       </c>
       <c r="H4" t="n">
@@ -2371,14 +2452,17 @@
         </is>
       </c>
       <c r="M4" t="n">
-        <v>4</v>
-      </c>
-      <c r="N4" t="inlineStr">
+        <v>6</v>
+      </c>
+      <c r="N4" t="n">
+        <v>6</v>
+      </c>
+      <c r="O4" t="inlineStr">
         <is>
           <t>2025-12-24</t>
         </is>
       </c>
-      <c r="O4" t="inlineStr">
+      <c r="P4" t="inlineStr">
         <is>
           <t>20251224</t>
         </is>
@@ -2417,7 +2501,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>+9.06%</t>
+          <t>+5.95%</t>
         </is>
       </c>
       <c r="H5" t="n">
@@ -2444,14 +2528,17 @@
         </is>
       </c>
       <c r="M5" t="n">
-        <v>4</v>
-      </c>
-      <c r="N5" t="inlineStr">
+        <v>6</v>
+      </c>
+      <c r="N5" t="n">
+        <v>6</v>
+      </c>
+      <c r="O5" t="inlineStr">
         <is>
           <t>2025-12-24</t>
         </is>
       </c>
-      <c r="O5" t="inlineStr">
+      <c r="P5" t="inlineStr">
         <is>
           <t>20251224</t>
         </is>
@@ -2490,7 +2577,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>+3.23%</t>
+          <t>+2.14%</t>
         </is>
       </c>
       <c r="H6" t="n">
@@ -2517,14 +2604,17 @@
         </is>
       </c>
       <c r="M6" t="n">
-        <v>4</v>
-      </c>
-      <c r="N6" t="inlineStr">
+        <v>6</v>
+      </c>
+      <c r="N6" t="n">
+        <v>6</v>
+      </c>
+      <c r="O6" t="inlineStr">
         <is>
           <t>2025-12-24</t>
         </is>
       </c>
-      <c r="O6" t="inlineStr">
+      <c r="P6" t="inlineStr">
         <is>
           <t>20251224</t>
         </is>
@@ -2541,7 +2631,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O6"/>
+  <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2617,10 +2707,15 @@
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
+          <t>Files Count</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
           <t>Analysis Date</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Data Date</t>
         </is>
@@ -2659,7 +2754,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>+21.66%</t>
+          <t>+16.98%</t>
         </is>
       </c>
       <c r="H2" t="n">
@@ -2686,14 +2781,17 @@
         </is>
       </c>
       <c r="M2" t="n">
-        <v>4</v>
-      </c>
-      <c r="N2" t="inlineStr">
+        <v>5</v>
+      </c>
+      <c r="N2" t="n">
+        <v>5</v>
+      </c>
+      <c r="O2" t="inlineStr">
         <is>
           <t>2025-12-24</t>
         </is>
       </c>
-      <c r="O2" t="inlineStr">
+      <c r="P2" t="inlineStr">
         <is>
           <t>20251223</t>
         </is>
@@ -2732,7 +2830,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>+259.97%</t>
+          <t>+134.88%</t>
         </is>
       </c>
       <c r="H3" t="n">
@@ -2759,14 +2857,17 @@
         </is>
       </c>
       <c r="M3" t="n">
-        <v>4</v>
-      </c>
-      <c r="N3" t="inlineStr">
+        <v>6</v>
+      </c>
+      <c r="N3" t="n">
+        <v>6</v>
+      </c>
+      <c r="O3" t="inlineStr">
         <is>
           <t>2025-12-24</t>
         </is>
       </c>
-      <c r="O3" t="inlineStr">
+      <c r="P3" t="inlineStr">
         <is>
           <t>20251224</t>
         </is>
@@ -2805,7 +2906,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>+240.85%</t>
+          <t>+126.49%</t>
         </is>
       </c>
       <c r="H4" t="n">
@@ -2832,14 +2933,17 @@
         </is>
       </c>
       <c r="M4" t="n">
-        <v>4</v>
-      </c>
-      <c r="N4" t="inlineStr">
+        <v>6</v>
+      </c>
+      <c r="N4" t="n">
+        <v>6</v>
+      </c>
+      <c r="O4" t="inlineStr">
         <is>
           <t>2025-12-24</t>
         </is>
       </c>
-      <c r="O4" t="inlineStr">
+      <c r="P4" t="inlineStr">
         <is>
           <t>20251224</t>
         </is>
@@ -2878,7 +2982,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>+5.55%</t>
+          <t>+3.66%</t>
         </is>
       </c>
       <c r="H5" t="n">
@@ -2905,14 +3009,17 @@
         </is>
       </c>
       <c r="M5" t="n">
-        <v>4</v>
-      </c>
-      <c r="N5" t="inlineStr">
+        <v>6</v>
+      </c>
+      <c r="N5" t="n">
+        <v>6</v>
+      </c>
+      <c r="O5" t="inlineStr">
         <is>
           <t>2025-12-24</t>
         </is>
       </c>
-      <c r="O5" t="inlineStr">
+      <c r="P5" t="inlineStr">
         <is>
           <t>20251224</t>
         </is>
@@ -2951,7 +3058,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>+64.91%</t>
+          <t>+39.58%</t>
         </is>
       </c>
       <c r="H6" t="n">
@@ -2978,14 +3085,17 @@
         </is>
       </c>
       <c r="M6" t="n">
-        <v>4</v>
-      </c>
-      <c r="N6" t="inlineStr">
+        <v>6</v>
+      </c>
+      <c r="N6" t="n">
+        <v>6</v>
+      </c>
+      <c r="O6" t="inlineStr">
         <is>
           <t>2025-12-24</t>
         </is>
       </c>
-      <c r="O6" t="inlineStr">
+      <c r="P6" t="inlineStr">
         <is>
           <t>20251224</t>
         </is>

</xml_diff>